<commit_message>
TFIDF dengan judul dan deskripsi
</commit_message>
<xml_diff>
--- a/res/Keywords.xlsx
+++ b/res/Keywords.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>makan</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>khasiat</t>
+  </si>
+  <si>
+    <t>bayi</t>
+  </si>
+  <si>
+    <t>fog</t>
   </si>
 </sst>
 </file>
@@ -395,6 +401,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>